<commit_message>
Added exception log, fixed typo in Monobank format, updated settings and template
</commit_message>
<xml_diff>
--- a/Finance.Formatter.Core/Templates/Template.xlsx
+++ b/Finance.Formatter.Core/Templates/Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrii.slobodianiuk\source\repos\Mono.Finance.Formatter\Finance.Formatter.Core\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82F947F-879C-4CF9-8C09-164F208E7D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BD6354-03D5-459F-A176-5D5AE3495CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>DateTime</t>
   </si>
@@ -92,12 +92,21 @@
   <si>
     <t>Кількість з USDEquivalent</t>
   </si>
+  <si>
+    <t>Static expenses:</t>
+  </si>
+  <si>
+    <t>Static Total:</t>
+  </si>
+  <si>
+    <t>All total:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,13 +114,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -133,7 +157,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
@@ -785,6 +809,20 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -18335,221 +18373,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D8C1A9C8-C5FB-4FC0-BE35-77153D9920F8}" name="Зведена таблиця1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="IsFop">
-  <location ref="A38:B39" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="13">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item m="1" x="1"/>
-        <item m="1" x="2"/>
-        <item h="1" x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="8"/>
-  </rowFields>
-  <rowItems count="1">
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Кількість з USDEquivalent" fld="6" subtotal="count" baseField="8" baseItem="0" numFmtId="10">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{E15A36E0-9728-4e99-A89B-3F7291B0FE68}">
-          <x14:dataField pivotShowAs="percentOfParentRow"/>
-        </ext>
-      </extLst>
-    </dataField>
-  </dataFields>
-  <chartFormats count="4">
-    <chartFormat chart="1" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="2">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleMedium14" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A7D34499-2DC9-4132-A8BD-E583DB85EEA7}" name="Зведена таблиця4" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Keyword">
-  <location ref="J38:K40" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="13">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="24">
-        <item m="1" x="1"/>
-        <item m="1" x="15"/>
-        <item m="1" x="11"/>
-        <item m="1" x="20"/>
-        <item m="1" x="2"/>
-        <item m="1" x="10"/>
-        <item m="1" x="21"/>
-        <item m="1" x="18"/>
-        <item m="1" x="5"/>
-        <item m="1" x="3"/>
-        <item m="1" x="9"/>
-        <item m="1" x="17"/>
-        <item m="1" x="8"/>
-        <item m="1" x="4"/>
-        <item m="1" x="19"/>
-        <item m="1" x="7"/>
-        <item m="1" x="16"/>
-        <item m="1" x="13"/>
-        <item m="1" x="6"/>
-        <item m="1" x="14"/>
-        <item m="1" x="12"/>
-        <item m="1" x="22"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="9"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x v="22"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Сума з USDEquivalent" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium14" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{40D18BA9-BAB6-4189-BEAA-9A64FF34EEEA}" name="Зведена таблиця5" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="F2:F3" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="13">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Сума з USDEquivalent" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{567A7815-FD1B-4C83-AC4F-9C3EA7730A51}" name="Зведена таблиця3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Category">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{567A7815-FD1B-4C83-AC4F-9C3EA7730A51}" name="Зведена таблиця3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Category">
   <location ref="G38:H40" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -18564,7 +18388,7 @@
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="13">
-        <item h="1" m="1" x="1"/>
+        <item m="1" x="1"/>
         <item m="1" x="8"/>
         <item m="1" x="3"/>
         <item m="1" x="2"/>
@@ -18622,8 +18446,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8D3A34E1-00F5-422B-9B44-E23047126B67}" name="Зведена таблиця2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Currency">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8D3A34E1-00F5-422B-9B44-E23047126B67}" name="Зведена таблиця2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Currency">
   <location ref="D38:E40" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -18725,6 +18549,229 @@
     </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleMedium14" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D8C1A9C8-C5FB-4FC0-BE35-77153D9920F8}" name="Зведена таблиця1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="IsFop">
+  <location ref="A38:B39" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item m="1" x="1"/>
+        <item m="1" x="2"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="8"/>
+  </rowFields>
+  <rowItems count="1">
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Кількість з USDEquivalent" fld="6" subtotal="count" baseField="8" baseItem="0" numFmtId="10">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{E15A36E0-9728-4e99-A89B-3F7291B0FE68}">
+          <x14:dataField pivotShowAs="percentOfParentRow"/>
+        </ext>
+      </extLst>
+    </dataField>
+  </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleMedium14" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A7D34499-2DC9-4132-A8BD-E583DB85EEA7}" name="Зведена таблиця4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Keyword">
+  <location ref="J38:K40" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="24">
+        <item m="1" x="1"/>
+        <item m="1" x="15"/>
+        <item m="1" x="11"/>
+        <item m="1" x="20"/>
+        <item m="1" x="2"/>
+        <item m="1" x="10"/>
+        <item m="1" x="21"/>
+        <item m="1" x="18"/>
+        <item m="1" x="5"/>
+        <item m="1" x="3"/>
+        <item m="1" x="9"/>
+        <item m="1" x="17"/>
+        <item m="1" x="8"/>
+        <item m="1" x="4"/>
+        <item m="1" x="19"/>
+        <item m="1" x="7"/>
+        <item m="1" x="16"/>
+        <item m="1" x="13"/>
+        <item m="1" x="6"/>
+        <item m="1" x="14"/>
+        <item m="1" x="12"/>
+        <item m="1" x="22"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="9"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x v="22"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Сума з USDEquivalent" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium14" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{40D18BA9-BAB6-4189-BEAA-9A64FF34EEEA}" name="Зведена таблиця5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значення" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F2:F3" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="13">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Сума з USDEquivalent" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
@@ -19026,8 +19073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5985AE3-C753-48B3-8A9B-27C3CF5C7EE6}">
   <dimension ref="A2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19043,13 +19090,36 @@
     <col min="11" max="11" width="19.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="6:8" x14ac:dyDescent="0.35">
       <c r="F2" t="s">
         <v>13</v>
       </c>
+      <c r="H2" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F3" s="4"/>
+    <row r="3" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F14">
+        <f>ABS(GETPIVOTDATA("USDEquivalent",$F$2))+H14</f>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f>SUM(H3:H12)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
@@ -19085,29 +19155,23 @@
       <c r="D39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E39" s="4"/>
       <c r="G39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H39" s="4"/>
       <c r="J39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K39" s="4"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E40" s="4"/>
       <c r="G40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H40" s="4"/>
       <c r="J40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K40" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>